<commit_message>
Fix checklist  titolo corretto (""CASO OK / KO"").
</commit_message>
<xml_diff>
--- a/report-checklist.xlsx
+++ b/report-checklist.xlsx
@@ -56,10 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="246">
-  <si>
-    <t xml:space="preserve">KO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="246">
   <si>
     <t xml:space="preserve">NOME FORNITORE:</t>
   </si>
@@ -139,7 +136,7 @@
     <t xml:space="preserve">NOTE</t>
   </si>
   <si>
-    <t xml:space="preserve">CASI OK / KO</t>
+    <t xml:space="preserve">CASO OK / KO</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE</t>
@@ -336,6 +333,9 @@
   "ts": "2023-04-27T13:47:08Z"
 } 
 L'operazione è bloccante non al fine della redazione della lettera ma al fine del processo di validazione e successiva firma digitale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KO</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
@@ -1275,7 +1275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1314,17 +1314,6 @@
         <color rgb="FFFFFFFF"/>
       </right>
       <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1404,7 +1393,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1477,8 +1466,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1486,26 +1475,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1513,15 +1498,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1529,15 +1514,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1545,11 +1530,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1712,14 +1697,14 @@
   <dimension ref="A1:T214"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="V10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="T10" activeCellId="0" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -1752,17 +1737,15 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="4"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="T1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="8"/>
       <c r="F2" s="2"/>
@@ -1783,11 +1766,11 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="11"/>
       <c r="F3" s="2"/>
@@ -1810,7 +1793,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="1"/>
@@ -1834,11 +1817,11 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1915,1070 +1898,1070 @@
     </row>
     <row r="9" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="K9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="N9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="O9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="P9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="Q9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="R9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="17" t="s">
+      <c r="S9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="T9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="18" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="E10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="21" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="22" t="n">
+      <c r="H10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="21" t="n">
         <v>45044</v>
       </c>
-      <c r="G10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="23" t="s">
+      <c r="G11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="26" t="s">
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="T10" s="6" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="21" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="21" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="n">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="B15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="22" t="n">
+      <c r="D15" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="n">
+        <v>45</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="n">
+        <v>63</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P17" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="n">
+        <v>64</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O18" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P18" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="n">
+        <v>65</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="n">
+        <v>66</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="27" t="n">
         <v>45044</v>
       </c>
-      <c r="G11" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" s="20" t="s">
+      <c r="G20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="O20" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P20" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18" t="n">
+        <v>67</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="22" t="n">
+      <c r="D21" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="O21" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P21" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="18" t="n">
+        <v>68</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="n">
+        <v>69</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="27" t="n">
+        <v>45043</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P23" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18" t="n">
+        <v>70</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="27" t="n">
         <v>45044</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" s="20" t="s">
+      <c r="G24" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="O24" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P24" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18" t="n">
+        <v>71</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="22" t="n">
+      <c r="D25" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="27" t="n">
         <v>45044</v>
       </c>
-      <c r="G13" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="n">
-        <v>29</v>
-      </c>
-      <c r="B14" s="20" t="s">
+      <c r="G25" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="O25" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="n">
+        <v>72</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O14" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="26" t="s">
+      <c r="D26" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="27" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="O26" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P26" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="T26" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="T14" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="n">
-        <v>37</v>
-      </c>
-      <c r="B15" s="20" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="18" t="n">
+        <v>73</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="n">
-        <v>45</v>
-      </c>
-      <c r="B16" s="20" t="s">
+      <c r="D27" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="27" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="T27" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="18" t="n">
+        <v>74</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="n">
+      <c r="D28" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="27" t="n">
+        <v>45044</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="O28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="T28" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P17" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="n">
-        <v>64</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="O18" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P18" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="T18" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="n">
-        <v>65</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="O19" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="T19" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="n">
-        <v>66</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="O20" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P20" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="T20" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="n">
-        <v>67</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="O21" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P21" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="T21" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="n">
-        <v>68</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="O22" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P22" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="n">
-        <v>69</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" s="28" t="n">
-        <v>45043</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N23" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="O23" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P23" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="T23" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="n">
-        <v>70</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M24" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N24" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="O24" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P24" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="n">
-        <v>71</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M25" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="O25" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P25" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="n">
-        <v>72</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M26" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="O26" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="P26" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="T26" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="n">
-        <v>73</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N27" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="O27" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P27" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="T27" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="n">
-        <v>74</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="F28" s="28" t="n">
-        <v>45044</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="J28" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M28" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="O28" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="P28" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="T28" s="6" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6177,14 +6160,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>163</v>
       </c>
     </row>
@@ -6222,7 +6205,7 @@
       <c r="A8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>170</v>
       </c>
     </row>
@@ -7251,7 +7234,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -7259,12 +7242,12 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>174</v>
       </c>
     </row>
@@ -7272,31 +7255,31 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="n">
+      <c r="A4" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="n">
+      <c r="A5" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="n">
+      <c r="A6" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="n">
+      <c r="A7" s="31" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -7304,50 +7287,50 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="n">
+      <c r="A8" s="34" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="n">
+      <c r="A9" s="36" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="n">
+      <c r="A10" s="36" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="n">
+      <c r="A11" s="36" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="n">
+      <c r="A12" s="36" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="n">
+      <c r="A13" s="36" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>184</v>
       </c>
     </row>
@@ -8365,7 +8348,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.86"/>
@@ -8376,10 +8359,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>185</v>
@@ -8389,688 +8372,688 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="40" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="40" t="n">
+      <c r="C10" s="39" t="n">
         <v>191</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C11" s="40" t="n">
+      <c r="C11" s="39" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="40" t="n">
+      <c r="C12" s="39" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C13" s="40" t="n">
+      <c r="C13" s="39" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="40" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C14" s="40" t="n">
+      <c r="C14" s="39" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="39" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C15" s="40" t="n">
+      <c r="C15" s="39" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="40" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="40" t="n">
+      <c r="C16" s="39" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="40" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="40" t="n">
+      <c r="C17" s="39" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="40" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="40" t="n">
+      <c r="C18" s="39" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="40" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="40" t="n">
+      <c r="C19" s="39" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="39" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C20" s="40" t="n">
+      <c r="C20" s="39" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="39" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C21" s="40" t="n">
+      <c r="C21" s="39" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="40" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C22" s="40" t="n">
+      <c r="C22" s="39" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="39" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C23" s="40" t="n">
+      <c r="C23" s="39" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="40" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="40" t="n">
+      <c r="C24" s="39" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="40" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C25" s="40" t="n">
+      <c r="C25" s="39" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="40" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C26" s="40" t="n">
+      <c r="C26" s="39" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="40" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C27" s="40" t="n">
+      <c r="C27" s="39" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="39" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="39" t="s">
+      <c r="A28" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C28" s="40" t="n">
+      <c r="C28" s="39" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="39" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C29" s="40" t="n">
+      <c r="C29" s="39" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="41" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C30" s="40" t="n">
+      <c r="C30" s="39" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="39" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C31" s="40" t="n">
+      <c r="C31" s="39" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="40" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C32" s="40" t="n">
+      <c r="C32" s="39" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="40" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C33" s="40" t="n">
+      <c r="C33" s="39" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="41" t="s">
+      <c r="D33" s="40" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C34" s="40" t="n">
+      <c r="C34" s="39" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="41" t="s">
+      <c r="D34" s="40" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="40" t="n">
+      <c r="C35" s="39" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="40" t="n">
+      <c r="D35" s="39" t="n">
         <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="39" t="s">
+      <c r="A36" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C36" s="40" t="n">
+      <c r="C36" s="39" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="40" t="n">
+      <c r="D36" s="39" t="n">
         <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C37" s="40" t="n">
+      <c r="C37" s="39" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="41" t="n">
+      <c r="D37" s="40" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C38" s="40" t="n">
+      <c r="C38" s="39" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="40" t="n">
+      <c r="D38" s="39" t="n">
         <v>252</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C39" s="40" t="n">
+      <c r="C39" s="39" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="41" t="n">
+      <c r="D39" s="40" t="n">
         <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C40" s="40" t="n">
+      <c r="C40" s="39" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="41" t="n">
+      <c r="D40" s="40" t="n">
         <v>284</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C41" s="40" t="n">
+      <c r="C41" s="39" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="41" t="n">
+      <c r="D41" s="40" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="C42" s="40" t="n">
+      <c r="C42" s="39" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="41" t="n">
+      <c r="D42" s="40" t="n">
         <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C43" s="40" t="n">
+      <c r="C43" s="39" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="40" t="n">
+      <c r="D43" s="39" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="39" t="s">
+      <c r="A44" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C44" s="40" t="n">
+      <c r="C44" s="39" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="40" t="n">
+      <c r="D44" s="39" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C45" s="40" t="n">
+      <c r="C45" s="39" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="41" t="n">
+      <c r="D45" s="40" t="n">
         <v>239</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C46" s="40" t="n">
+      <c r="C46" s="39" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="40" t="n">
+      <c r="D46" s="39" t="n">
         <v>255</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C47" s="40" t="n">
+      <c r="C47" s="39" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="41" t="n">
+      <c r="D47" s="40" t="n">
         <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C48" s="40" t="n">
+      <c r="C48" s="39" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="41" t="n">
+      <c r="D48" s="40" t="n">
         <v>287</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C49" s="40" t="n">
+      <c r="C49" s="39" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="41" t="n">
+      <c r="D49" s="40" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="C50" s="40" t="n">
+      <c r="C50" s="39" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="41" t="n">
+      <c r="D50" s="40" t="n">
         <v>319</v>
       </c>
     </row>
@@ -10054,7 +10037,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -10063,10 +10046,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Aggiornati gestione errore 29,37,45,63,65,72,74
</commit_message>
<xml_diff>
--- a/report-checklist.xlsx
+++ b/report-checklist.xlsx
@@ -318,7 +318,8 @@
     <t xml:space="preserve">Validazione fallita. Contattare l'assistenza o attendere la correzione. </t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il campo del token JWT oggetto dell'errore non viene valorizzato</t>
+    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il campo del token JWT oggetto dell'errore non viene valorizzato.
+Corretto l’eventuale errore, in Backoffice viene tentata nuovamente la validazione, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -397,7 +398,26 @@
     <t xml:space="preserve">8926cf9cbde14cfd</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il campo del token JWT oggetto dell'errore viene valorizzato in modo errato</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il campo del token JWT oggetto dell'errore viene valorizzato in modo errato
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Corretto l’eventuale errore, in Backoffice viene tentata nuovamente la validazione, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -421,7 +441,26 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene segnalato all'utente un errore di timeout, chiedendo conferma se proseguire con la validazione del documento o riprovare più tardi</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene segnalato all'utente un errore di timeout, chiedendo conferma se proseguire con la validazione del documento o riprovare più tardi.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> Viene tentata nuovamente la validazione attraverso una coda di retry, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -441,7 +480,26 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.6b981b6800^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il confidentiality code oggetto dell'errore non viene valorizzato</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il confidentiality code oggetto dell'errore non viene valorizzato.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Successivamente alla correzione, viene tentata nuovamente la validazione in backoffice, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -514,7 +572,27 @@
     <t xml:space="preserve">Validazione fallita. Il livello di riservatezza del documento (Restricted) non è compatibile con la lettera di dimissione. Contattare l'assistenza o attendere la correzione. </t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il confidentiality code oggetto dell'errore non viene valorizzato correttamente</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa software per cui il confidentiality code oggetto dell'errore non viene valorizzato correttamente
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">
+Successivamente alla correzione e verifica del confidentialycode che sia N o V a seconda della tipologia di documento, viene tentata nuovamente la validazione in backoffice, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -789,7 +867,27 @@
     <t xml:space="preserve">Validazione fallita. Nella sezione Motivo del Ricovero le diagnosi non sono codificate correttamente. Contattare l'assistenza o attendere la correzione. </t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa per cui il dizionario delle diagnosi non è valorizzato correttamente</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa per cui il dizionario delle diagnosi non è valorizzato correttamente
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">
+Successivamente alla correzione del dizionario, viene avvisato l’operatore di correggere la lettera attingendo al dizionario aggiornato, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -826,7 +924,26 @@
     <t xml:space="preserve">Validazione fallita. Nella sezione Terapia Farmacologica alla dimissione le vie di somministrazione non sono codificate correttamente. Contattare l'assistenza o attendere la correzione. </t>
   </si>
   <si>
-    <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa per cui il dizionario delle vie di somministrazione non è valorizzato correttamente</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Viene generato un log che riporta i dettagli sull'errore contenuti nella response. In backoffice si va a verificare la causa per cui il dizionario delle vie di somministrazione non è valorizzato correttamente
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Successivamente alla correzione del dizionario, viene avvisato l’operatore di correggere la lettera attingendo al dizionario aggiornato, se la validazione va a buon fine, l’LDO viene posta in uno stato validata pronta da firmare e viene notificata tramite interfaccia apposita al medico che effettuera la firma e l’invio per la pubblicazione nel FSE</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -1181,7 +1298,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1228,6 +1345,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1510,7 +1633,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1542,7 +1665,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1696,15 +1819,15 @@
   </sheetPr>
   <dimension ref="A1:T214"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="V10" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V1" activeCellId="0" sqref="V1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T10" activeCellId="0" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="Q28" activeCellId="0" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -2142,7 +2265,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="254.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="n">
         <v>29</v>
       </c>
@@ -2198,7 +2321,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="254.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="n">
         <v>37</v>
       </c>
@@ -2254,7 +2377,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="215.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="n">
         <v>45</v>
       </c>
@@ -2292,7 +2415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="282.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="n">
         <v>63</v>
       </c>
@@ -2404,7 +2527,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="322.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="n">
         <v>65</v>
       </c>
@@ -2852,7 +2975,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="282.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="n">
         <v>73</v>
       </c>
@@ -2908,7 +3031,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="273.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="n">
         <v>74</v>
       </c>
@@ -6156,11 +6279,11 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="8.85"/>
@@ -7230,11 +7353,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -8342,13 +8465,13 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.86"/>
@@ -10033,11 +10156,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>

</xml_diff>

<commit_message>
aggiornato report-checklist.xslx - 7 29.09.2023
aggiornato report-checklist.xslx - 7 29.09.2023
</commit_message>
<xml_diff>
--- a/report-checklist.xlsx
+++ b/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">Viene visualizzata la risposta del gateway+Viene avvisato l’inviante che c’e’ un errore strutturale e di avvisare il fornitore del software l’errore non inficia la creazione del referto in quanto la trasmissione e’ posteriore+ viene registrata in un file di log+la richiesta viene inserita tra quelle da ritrasmettere</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene rilevata la segnalazione da parte dell’inviante e corretto l’errore del software da parte di Datasoft</t>
+    <t xml:space="preserve">Apertura di ticket e analisi del log</t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -555,7 +555,7 @@
     <t xml:space="preserve">Viene segnalato all’INVIANTE che si e’ verificato un TIMEOUT e puo’ provare a ritentare e a controllare lo stato della connessione internet +  l’evento viene registrato nel log+la richiesta viene inserita tra quelle da ritrasmettere+se l’operazione non e’ interattiva, l’inviante consulta il log</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene chiesto all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
+    <t xml:space="preserve">Viene suggerito all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT6_KO</t>
@@ -654,10 +654,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.092424a8b83ac1734d0e118a4c3a43c793f3f6c63b6ba838d480115903a3b457.0e8346143a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All’INVIANTE viene visualizzata la risposta del Gateway.+Richiesta di contattare il fornitore del software.</t>
+    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log+richiesta di contattare il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -684,9 +681,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.687d9ade5891f6681a5a8231ce0d4ac16be6cb2e3ab9e2b490ad662dff2b34fa.a9ea1d1558^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’errore viene gestito richiedendo all’INVIANTE di contattare il fornitore del software, dato che si tratta di una situazione anomala che non puo’ dipendere da qualche sua azione+la richiesta viene inserita tra quelle da ritrasmettere</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -2075,9 +2069,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>939600</xdr:rowOff>
+      <xdr:rowOff>939240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2087,7 +2081,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5370840" cy="2889360"/>
+          <a:ext cx="5370480" cy="2889000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4330,11 +4324,11 @@
   <dimension ref="A1:T959"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="O27" activeCellId="0" sqref="O27"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5318,7 +5312,7 @@
         <v>56</v>
       </c>
       <c r="P26" s="32" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="Q26" s="32"/>
       <c r="R26" s="33"/>
@@ -5338,10 +5332,10 @@
         <v>49</v>
       </c>
       <c r="D27" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>129</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
@@ -5351,7 +5345,7 @@
         <v>92</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
@@ -5376,22 +5370,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>131</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>132</v>
       </c>
       <c r="F28" s="30" t="n">
         <v>45082</v>
       </c>
       <c r="G28" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>134</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>135</v>
       </c>
       <c r="J28" s="32" t="s">
         <v>56</v>
@@ -5410,7 +5404,7 @@
         <v>56</v>
       </c>
       <c r="P28" s="32" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="Q28" s="32"/>
       <c r="R28" s="33"/>
@@ -17041,10 +17035,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17052,125 +17046,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>145</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="38" t="s">
         <v>148</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>151</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="39" t="s">
         <v>157</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="39" t="s">
         <v>160</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>163</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17178,111 +17172,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17290,111 +17284,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17402,111 +17396,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17514,7 +17508,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C35" s="38" t="n">
         <v>195</v>
@@ -17525,10 +17519,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C36" s="38" t="n">
         <v>211</v>
@@ -17539,10 +17533,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C37" s="38" t="n">
         <v>227</v>
@@ -17553,10 +17547,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C38" s="38" t="n">
         <v>243</v>
@@ -17567,10 +17561,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C39" s="38" t="n">
         <v>259</v>
@@ -17581,10 +17575,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C40" s="38" t="n">
         <v>275</v>
@@ -17595,10 +17589,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C41" s="38" t="n">
         <v>291</v>
@@ -17609,10 +17603,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C42" s="38" t="n">
         <v>307</v>
@@ -17626,7 +17620,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C43" s="38" t="n">
         <v>196</v>
@@ -17637,10 +17631,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C44" s="38" t="n">
         <v>212</v>
@@ -17651,10 +17645,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C45" s="38" t="n">
         <v>228</v>
@@ -17665,10 +17659,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C46" s="38" t="n">
         <v>244</v>
@@ -17679,10 +17673,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C47" s="38" t="n">
         <v>260</v>
@@ -17693,10 +17687,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C48" s="38" t="n">
         <v>276</v>
@@ -17707,10 +17701,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C49" s="38" t="n">
         <v>292</v>
@@ -17721,10 +17715,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C50" s="38" t="n">
         <v>308</v>
@@ -18723,7 +18717,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>56</v>
@@ -18731,7 +18725,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
report - 10 29.09.2023
report - 10 29.09.2023
</commit_message>
<xml_diff>
--- a/report-checklist.xlsx
+++ b/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="194">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -461,7 +461,7 @@
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway+Viene avvisato l’inviante che c’e’ un errore strutturale e di avvisare il fornitore del software l’errore non inficia la creazione del referto in quanto la trasmissione e’ posteriore+ viene registrata in un file di log+la richiesta viene inserita tra quelle da ritrasmettere</t>
+    <t xml:space="preserve">Errore dell’applicativo contattare  il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">Apertura di ticket e analisi del log</t>
@@ -542,9 +542,6 @@
     <t xml:space="preserve">a0fc8f87aabeb7ba</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_LAB_TIMEOUT</t>
   </si>
   <si>
@@ -552,7 +549,7 @@
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene segnalato all’INVIANTE che si e’ verificato un TIMEOUT e puo’ provare a ritentare e a controllare lo stato della connessione internet +  l’evento viene registrato nel log+la richiesta viene inserita tra quelle da ritrasmettere+se l’operazione non e’ interattiva, l’inviante consulta il log</t>
+    <t xml:space="preserve">Tineout riprovare piu’ tardi e controllare la connessione internet</t>
   </si>
   <si>
     <t xml:space="preserve">Viene suggerito all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
@@ -563,6 +560,9 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Non è possibile produrre un referto per i pazienti senza confidentiality code</t>
@@ -652,9 +652,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.092424a8b83ac1734d0e118a4c3a43c793f3f6c63b6ba838d480115903a3b457.0e8346143a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log+richiesta di contattare il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -872,7 +869,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1168,6 +1165,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1759,7 +1762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1909,6 +1912,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2069,9 +2076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>939240</xdr:rowOff>
+      <xdr:rowOff>938880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2081,7 +2088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5370480" cy="2889000"/>
+          <a:ext cx="5370120" cy="2888640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4324,11 +4331,11 @@
   <dimension ref="A1:T959"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P18" activeCellId="0" sqref="P18"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4905,7 +4912,7 @@
         <v>85</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="P16" s="32" t="s">
         <v>86</v>
@@ -4917,7 +4924,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="n">
         <v>44</v>
       </c>
@@ -4928,10 +4935,10 @@
         <v>49</v>
       </c>
       <c r="D17" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
@@ -4948,13 +4955,13 @@
         <v>56</v>
       </c>
       <c r="N17" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="32" t="s">
         <v>95</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P17" s="32" t="s">
-        <v>96</v>
       </c>
       <c r="Q17" s="32"/>
       <c r="R17" s="33"/>
@@ -4974,17 +4981,17 @@
         <v>49</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>97</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>98</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
       <c r="J18" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K18" s="32" t="s">
         <v>99</v>
@@ -5022,7 +5029,7 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
       <c r="J19" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K19" s="32" t="s">
         <v>102</v>
@@ -5060,7 +5067,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
       <c r="J20" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>105</v>
@@ -5098,7 +5105,7 @@
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
       <c r="J21" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K21" s="37" t="s">
         <v>108</v>
@@ -5136,7 +5143,7 @@
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K22" s="32" t="s">
         <v>111</v>
@@ -5174,7 +5181,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>114</v>
@@ -5212,7 +5219,7 @@
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>117</v>
@@ -5250,7 +5257,7 @@
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K25" s="32" t="s">
         <v>120</v>
@@ -5306,7 +5313,7 @@
         <v>56</v>
       </c>
       <c r="N26" s="32" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="O26" s="32" t="s">
         <v>56</v>
@@ -5332,20 +5339,20 @@
         <v>49</v>
       </c>
       <c r="D27" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>128</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
       <c r="J27" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
@@ -5370,22 +5377,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>130</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>131</v>
       </c>
       <c r="F28" s="30" t="n">
         <v>45082</v>
       </c>
       <c r="G28" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>133</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>134</v>
       </c>
       <c r="J28" s="32" t="s">
         <v>56</v>
@@ -5397,8 +5404,8 @@
       <c r="M28" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="N28" s="32" t="s">
-        <v>126</v>
+      <c r="N28" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="O28" s="32" t="s">
         <v>56</v>
@@ -17035,10 +17042,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17046,125 +17053,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>138</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>141</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="40" t="s">
         <v>144</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="39" t="s">
         <v>147</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="40" t="s">
         <v>150</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="40" t="s">
         <v>153</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="40" t="s">
         <v>156</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="40" t="s">
         <v>159</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="39" t="s">
+      <c r="D10" s="39" t="s">
         <v>162</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17172,111 +17179,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="39" t="n">
+        <v>192</v>
+      </c>
+      <c r="D11" s="39" t="s">
         <v>164</v>
-      </c>
-      <c r="C11" s="38" t="n">
-        <v>192</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C12" s="39" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>166</v>
+      <c r="D12" s="39" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C13" s="39" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="39" t="s">
-        <v>167</v>
+      <c r="D13" s="40" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C14" s="39" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>168</v>
+      <c r="D14" s="39" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C15" s="39" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="39" t="s">
-        <v>169</v>
+      <c r="D15" s="40" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C16" s="39" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="39" t="s">
-        <v>170</v>
+      <c r="D16" s="40" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C17" s="39" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="39" t="s">
-        <v>171</v>
+      <c r="D17" s="40" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C18" s="39" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>172</v>
+      <c r="D18" s="40" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17284,111 +17291,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="39" t="n">
+        <v>193</v>
+      </c>
+      <c r="D19" s="39" t="s">
         <v>173</v>
-      </c>
-      <c r="C19" s="38" t="n">
-        <v>193</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C20" s="39" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>175</v>
+      <c r="D20" s="39" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C21" s="39" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="39" t="s">
-        <v>176</v>
+      <c r="D21" s="40" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C22" s="39" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>177</v>
+      <c r="D22" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C23" s="39" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="39" t="s">
-        <v>178</v>
+      <c r="D23" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C24" s="39" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="39" t="s">
-        <v>179</v>
+      <c r="D24" s="40" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C25" s="39" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="39" t="s">
-        <v>180</v>
+      <c r="D25" s="40" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C26" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C26" s="39" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="39" t="s">
-        <v>181</v>
+      <c r="D26" s="40" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17396,111 +17403,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="39" t="n">
+        <v>194</v>
+      </c>
+      <c r="D27" s="39" t="s">
         <v>182</v>
-      </c>
-      <c r="C27" s="38" t="n">
-        <v>194</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C28" s="39" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="38" t="s">
-        <v>184</v>
+      <c r="D28" s="39" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C29" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C29" s="39" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="40" t="s">
-        <v>185</v>
+      <c r="D29" s="41" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C30" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C30" s="39" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="38" t="s">
-        <v>186</v>
+      <c r="D30" s="39" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C31" s="39" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="39" t="s">
-        <v>187</v>
+      <c r="D31" s="40" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C32" s="39" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="39" t="s">
-        <v>188</v>
+      <c r="D32" s="40" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C33" s="39" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="39" t="s">
-        <v>189</v>
+      <c r="D33" s="40" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C34" s="39" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="39" t="s">
-        <v>190</v>
+      <c r="D34" s="40" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17508,110 +17515,110 @@
         <v>49</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C35" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C35" s="39" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="38" t="n">
+      <c r="D35" s="39" t="n">
         <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C36" s="39" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="38" t="n">
+      <c r="D36" s="39" t="n">
         <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C37" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C37" s="39" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="39" t="n">
+      <c r="D37" s="40" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C38" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C38" s="39" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="38" t="n">
+      <c r="D38" s="39" t="n">
         <v>252</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C39" s="39" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="39" t="n">
+      <c r="D39" s="40" t="n">
         <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C40" s="39" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="39" t="n">
+      <c r="D40" s="40" t="n">
         <v>284</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C41" s="39" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="39" t="n">
+      <c r="D41" s="40" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C42" s="39" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="39" t="n">
+      <c r="D42" s="40" t="n">
         <v>316</v>
       </c>
     </row>
@@ -17620,110 +17627,110 @@
         <v>49</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C43" s="39" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="38" t="n">
+      <c r="D43" s="39" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C44" s="39" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="38" t="n">
+      <c r="D44" s="39" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C45" s="39" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="39" t="n">
+      <c r="D45" s="40" t="n">
         <v>239</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C46" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C46" s="39" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="38" t="n">
+      <c r="D46" s="39" t="n">
         <v>255</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C47" s="39" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="39" t="n">
+      <c r="D47" s="40" t="n">
         <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C48" s="39" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="39" t="n">
+      <c r="D48" s="40" t="n">
         <v>287</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C49" s="39" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="39" t="n">
+      <c r="D49" s="40" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C50" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C50" s="39" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="39" t="n">
+      <c r="D50" s="40" t="n">
         <v>319</v>
       </c>
     </row>
@@ -18708,27 +18715,27 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>92</v>
+      <c r="B3" s="42" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>